<commit_message>
Dodałem wagi Procesów do Bazy Danych, ułatwi to obliczanie pozycji na planszy konkurencji oraz sprawi że GM będzie mógł dostosować wagi
</commit_message>
<xml_diff>
--- a/backend/Initializers/DigitalWars_InicjalizacjaBazyDanych.xlsx
+++ b/backend/Initializers/DigitalWars_InicjalizacjaBazyDanych.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repozytoria\Projekt Zespołowy\ITM_ProjektZespo-owy\backend\Initializers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F73BB9-D68C-4678-AD7B-B7C0682EE7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDBC5C9-1B6A-4A25-8DAA-1BB2ECDA2019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="21" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="197">
   <si>
     <t>Stworzenie profilu organizacji</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t>#404040</t>
+  </si>
+  <si>
+    <t>ProcessWeight</t>
   </si>
 </sst>
 </file>
@@ -3023,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203EA4C9-990F-4F3C-8834-562941A4A0C3}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3034,9 +3037,10 @@
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>174</v>
       </c>
@@ -3050,10 +3054,13 @@
         <v>189</v>
       </c>
       <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3067,10 +3074,13 @@
         <v>190</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.17</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3084,10 +3094,13 @@
         <v>191</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0.13</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3101,10 +3114,13 @@
         <v>193</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.16</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3118,10 +3134,13 @@
         <v>194</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.22</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3135,10 +3154,13 @@
         <v>195</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>0.18</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3152,10 +3174,13 @@
         <v>192</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3169,10 +3194,13 @@
         <v>190</v>
       </c>
       <c r="E8">
+        <v>0.17</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3186,10 +3214,13 @@
         <v>191</v>
       </c>
       <c r="E9">
+        <v>0.13</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3203,10 +3234,13 @@
         <v>193</v>
       </c>
       <c r="E10">
+        <v>0.16</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3220,10 +3254,13 @@
         <v>194</v>
       </c>
       <c r="E11">
+        <v>0.22</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3237,10 +3274,13 @@
         <v>195</v>
       </c>
       <c r="E12">
+        <v>0.18</v>
+      </c>
+      <c r="F12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3254,10 +3294,13 @@
         <v>192</v>
       </c>
       <c r="E13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3271,10 +3314,13 @@
         <v>190</v>
       </c>
       <c r="E14">
+        <v>0.17</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3288,10 +3334,13 @@
         <v>191</v>
       </c>
       <c r="E15">
+        <v>0.13</v>
+      </c>
+      <c r="F15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3305,10 +3354,13 @@
         <v>193</v>
       </c>
       <c r="E16">
+        <v>0.16</v>
+      </c>
+      <c r="F16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3322,10 +3374,13 @@
         <v>194</v>
       </c>
       <c r="E17">
+        <v>0.22</v>
+      </c>
+      <c r="F17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3339,10 +3394,13 @@
         <v>195</v>
       </c>
       <c r="E18">
+        <v>0.18</v>
+      </c>
+      <c r="F18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3356,6 +3414,9 @@
         <v>192</v>
       </c>
       <c r="E19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F19">
         <v>3</v>
       </c>
     </row>
@@ -14616,8 +14677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="R172" sqref="R172"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection sqref="A1:H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Zmieniłem nazewnictwo przedwiotów w CardId. Dodałem endpointy do pobierania mapy enablerów i ostatnio zagranej karty przez stoły (w zależności od tego czy wyszukujemy po GameId czy po GameId i TeamId, dla GameId zwrócona zostanie lista dla GameId i TeamId zostanie swrócona jedna liczba)
</commit_message>
<xml_diff>
--- a/backend/Initializers/DigitalWars_InicjalizacjaBazyDanych.xlsx
+++ b/backend/Initializers/DigitalWars_InicjalizacjaBazyDanych.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ITM_ProjektZespo-owy-Grupson_Project\backend\Initializers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repozytoria\Projekt Zespołowy\ITM_ProjektZespo-owy\backend\Initializers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AA937F-9D36-4134-8791-95C496B77CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C5D73A-83E4-4CCE-8D0F-BEACE7A5626A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="21" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="208">
   <si>
     <t>Stworzenie profilu organizacji</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Podstawowy</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>DecisionBaseCost</t>
   </si>
   <si>
@@ -658,6 +655,12 @@
   </si>
   <si>
     <t>Zespół spędza więcej czasu na naprawianiu starych błędów, niż na wdrażaniu nowych rozwiązań, co spowalnia tempo całej transformacji. Dwa następne poruszenia na planszy będą o 50% krótsze.</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Hardware</t>
   </si>
 </sst>
 </file>
@@ -1158,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection sqref="A1:H61"/>
+    <sheetView topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1180,7 +1183,7 @@
         <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>107</v>
@@ -8642,19 +8645,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
         <v>174</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
-        <v>176</v>
-      </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F1" t="s">
         <v>107</v>
@@ -8665,13 +8668,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2">
         <v>0.17</v>
@@ -8685,13 +8688,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3">
         <v>0.13</v>
@@ -8705,13 +8708,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4">
         <v>0.16</v>
@@ -8725,13 +8728,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5">
         <v>0.22</v>
@@ -8745,13 +8748,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
         <v>187</v>
       </c>
-      <c r="C6" t="s">
-        <v>188</v>
-      </c>
       <c r="D6" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E6">
         <v>0.18</v>
@@ -8765,13 +8768,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7">
         <v>0.14000000000000001</v>
@@ -8785,13 +8788,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8">
         <v>0.17</v>
@@ -8805,13 +8808,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9">
         <v>0.13</v>
@@ -8825,13 +8828,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10">
         <v>0.16</v>
@@ -8845,13 +8848,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11">
         <v>0.22</v>
@@ -8865,13 +8868,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
         <v>187</v>
       </c>
-      <c r="C12" t="s">
-        <v>188</v>
-      </c>
       <c r="D12" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12">
         <v>0.18</v>
@@ -8885,13 +8888,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13">
         <v>0.14000000000000001</v>
@@ -8905,13 +8908,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14">
         <v>0.17</v>
@@ -8925,13 +8928,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15">
         <v>0.13</v>
@@ -8945,13 +8948,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16">
         <v>0.16</v>
@@ -8965,13 +8968,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E17">
         <v>0.22</v>
@@ -8985,13 +8988,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" t="s">
         <v>187</v>
       </c>
-      <c r="C18" t="s">
-        <v>188</v>
-      </c>
       <c r="D18" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18">
         <v>0.18</v>
@@ -9005,13 +9008,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19">
         <v>0.14000000000000001</v>
@@ -9029,7 +9032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB49C299-DBF3-4B16-B8E3-43150597C2A9}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -9043,27 +9046,27 @@
     <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>198</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>199</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>149</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>119</v>
@@ -9077,10 +9080,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>202</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24">
@@ -9098,10 +9101,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>204</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24">
@@ -9119,10 +9122,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24">
@@ -9142,10 +9145,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>202</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
@@ -9165,10 +9168,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>204</v>
       </c>
       <c r="D6" s="24">
         <v>1</v>
@@ -9188,10 +9191,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>205</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
@@ -9213,10 +9216,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>202</v>
       </c>
       <c r="D8" s="24">
         <v>2</v>
@@ -9236,10 +9239,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>204</v>
       </c>
       <c r="D9" s="24">
         <v>2</v>
@@ -9259,10 +9262,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>205</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="D10" s="24">
         <v>2</v>
@@ -9291,8 +9294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185C019C-5082-4509-8B3F-A49CA6E5A33C}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9393,7 +9396,7 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -9401,7 +9404,7 @@
         <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -9409,7 +9412,7 @@
         <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -9417,7 +9420,7 @@
         <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -9425,7 +9428,7 @@
         <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -9433,7 +9436,7 @@
         <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -9441,7 +9444,7 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -9449,7 +9452,7 @@
         <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -9457,7 +9460,7 @@
         <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -9465,7 +9468,7 @@
         <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -9473,7 +9476,7 @@
         <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -9481,7 +9484,7 @@
         <v>112</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -9489,7 +9492,7 @@
         <v>201</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -9497,7 +9500,7 @@
         <v>202</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -9505,7 +9508,7 @@
         <v>203</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -9513,7 +9516,7 @@
         <v>204</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -9521,7 +9524,7 @@
         <v>205</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -9529,7 +9532,7 @@
         <v>206</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -9537,7 +9540,7 @@
         <v>207</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -9545,7 +9548,7 @@
         <v>208</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -9553,7 +9556,7 @@
         <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -9561,7 +9564,7 @@
         <v>210</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -9569,7 +9572,7 @@
         <v>211</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -9577,7 +9580,7 @@
         <v>212</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -9585,7 +9588,7 @@
         <v>213</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -9593,7 +9596,7 @@
         <v>214</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -9601,7 +9604,7 @@
         <v>215</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -9609,7 +9612,7 @@
         <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -9617,7 +9620,7 @@
         <v>217</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -9625,7 +9628,7 @@
         <v>218</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -9633,7 +9636,7 @@
         <v>219</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -9641,7 +9644,7 @@
         <v>220</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -9649,7 +9652,7 @@
         <v>221</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -9657,7 +9660,7 @@
         <v>222</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -9665,7 +9668,7 @@
         <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -9709,10 +9712,10 @@
         <v>107</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1">
@@ -13119,8 +13122,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -13147,18 +13150,18 @@
         <v>107</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>101</v>
+      <c r="B2" s="16">
+        <v>201</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -13180,8 +13183,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>102</v>
+      <c r="B3" s="16">
+        <v>202</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>22</v>
@@ -13203,8 +13206,8 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>103</v>
+      <c r="B4" s="17">
+        <v>203</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>24</v>
@@ -13226,8 +13229,8 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>104</v>
+      <c r="B5" s="16">
+        <v>204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
@@ -13249,8 +13252,8 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>105</v>
+      <c r="B6" s="16">
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -13272,8 +13275,8 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>106</v>
+      <c r="B7" s="17">
+        <v>206</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -13295,8 +13298,8 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>107</v>
+      <c r="B8" s="16">
+        <v>207</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -13318,8 +13321,8 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>108</v>
+      <c r="B9" s="16">
+        <v>208</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
@@ -13341,8 +13344,8 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>109</v>
+      <c r="B10" s="17">
+        <v>209</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>36</v>
@@ -13364,8 +13367,8 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>110</v>
+      <c r="B11" s="16">
+        <v>210</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>38</v>
@@ -13387,8 +13390,8 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>111</v>
+      <c r="B12" s="16">
+        <v>211</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
@@ -13410,8 +13413,8 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>112</v>
+      <c r="B13" s="17">
+        <v>212</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>42</v>
@@ -13434,7 +13437,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="16">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>44</v>
@@ -13457,7 +13460,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="16">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>46</v>
@@ -13480,7 +13483,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="17">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>48</v>
@@ -13503,7 +13506,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>50</v>
@@ -13526,7 +13529,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="16">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>52</v>
@@ -13549,7 +13552,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="17">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
@@ -13572,7 +13575,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="16">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>56</v>
@@ -13595,7 +13598,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="16">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>58</v>
@@ -13617,8 +13620,8 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="17">
-        <v>209</v>
+      <c r="B22" s="16">
+        <v>221</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>60</v>
@@ -13641,7 +13644,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>62</v>
@@ -13663,8 +13666,8 @@
       <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="16">
-        <v>211</v>
+      <c r="B24" s="17">
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>64</v>
@@ -13687,7 +13690,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="17">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>66</v>
@@ -13709,8 +13712,8 @@
       <c r="A26" s="12">
         <v>25</v>
       </c>
-      <c r="B26" s="16">
-        <v>213</v>
+      <c r="B26" s="17">
+        <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>68</v>
@@ -13732,8 +13735,8 @@
       <c r="A27" s="12">
         <v>26</v>
       </c>
-      <c r="B27" s="16">
-        <v>214</v>
+      <c r="B27" s="17">
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>70</v>
@@ -13756,7 +13759,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="17">
-        <v>215</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>72</v>
@@ -13778,8 +13781,8 @@
       <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="16">
-        <v>216</v>
+      <c r="B29" s="17">
+        <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>74</v>
@@ -13801,8 +13804,8 @@
       <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="16">
-        <v>217</v>
+      <c r="B30" s="17">
+        <v>107</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>76</v>
@@ -13825,7 +13828,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="17">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>78</v>
@@ -13847,8 +13850,8 @@
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="16">
-        <v>219</v>
+      <c r="B32" s="17">
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>80</v>
@@ -13870,8 +13873,8 @@
       <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" s="16">
-        <v>220</v>
+      <c r="B33" s="17">
+        <v>110</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>82</v>
@@ -13893,8 +13896,8 @@
       <c r="A34" s="12">
         <v>33</v>
       </c>
-      <c r="B34" s="16">
-        <v>221</v>
+      <c r="B34" s="17">
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>84</v>
@@ -13916,8 +13919,8 @@
       <c r="A35" s="12">
         <v>34</v>
       </c>
-      <c r="B35" s="16">
-        <v>222</v>
+      <c r="B35" s="17">
+        <v>112</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>86</v>
@@ -20144,7 +20147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEC1AC8-2093-4D23-9D9C-37D51A2AA2D4}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -20237,19 +20240,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="G3" s="18">
         <v>8</v>
@@ -20345,19 +20348,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="G6" s="18">
         <v>8</v>
@@ -20459,19 +20462,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="G9" s="18">
         <v>8</v>

</xml_diff>